<commit_message>
Feat: intialization and get data process
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jana\Documents\Jana2023\CnaeProcess\CnaeIgbeProcesses\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -159,13 +158,19 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
+    <t>CNAE_URL</t>
+  </si>
+  <si>
+    <t>https://cnae.ibge.gov.br/?view=estrutura</t>
+  </si>
+  <si>
+    <t>cnaeactivities</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -534,11 +539,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -588,7 +593,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -615,7 +620,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1616,7 +1628,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2779,10 +2791,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>

<commit_message>
Fix: Update UiPath activities names and descriptions
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jana\Documents\Jana2023\CnaeProcess\CnaeIgbeProcesses\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Jana2023\CnaeProcess\CnaeIgbeProcesses\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD2B778-CDBB-4C52-9A46-41CFE30D229D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -165,13 +166,25 @@
   </si>
   <si>
     <t>cnaeactivities</t>
+  </si>
+  <si>
+    <t>PATH_PYTHON</t>
+  </si>
+  <si>
+    <t>LIBRARY_PATH_PYTHON</t>
+  </si>
+  <si>
+    <t>C:\Users\{NomeUsuárioWindows}\AppData\Local\Programs\Python\Python310</t>
+  </si>
+  <si>
+    <t>C:\Users\{NomeUsuárioWindows}\AppData\Local\Programs\Python\Python310\python310.dll</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -190,6 +203,13 @@
       <charset val="128"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -216,16 +236,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,17 +560,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5546875" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="2" max="2" width="79.6640625" customWidth="1"/>
     <col min="3" max="3" width="81.44140625" customWidth="1"/>
     <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
@@ -628,14 +649,32 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="B11" s="5"/>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="B14" s="5"/>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
@@ -1628,7 +1667,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2791,7 +2830,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>